<commit_message>
[MS08072024DS] - Added a question in arrays LongestConsecutiveSequence
</commit_message>
<xml_diff>
--- a/resources/sheets/data-structures.xlsx
+++ b/resources/sheets/data-structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHAKIR\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasmo4a\workspace-pasmo4a\docs\data-structures\resources\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26A68E7-146A-4C2E-AD64-69CAC85F997A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC73179-3A6B-41AD-B32E-07C76F637E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Question</t>
   </si>
@@ -579,7 +579,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,8 +782,12 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,8 +797,12 @@
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -804,8 +812,12 @@
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[MS12092024DS] - Added few Binary tree problems
</commit_message>
<xml_diff>
--- a/resources/sheets/data-structures.xlsx
+++ b/resources/sheets/data-structures.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasmo4a\workspace-pasmo4a\docs\data-structures\resources\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC73179-3A6B-41AD-B32E-07C76F637E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33474140-0750-44CD-A916-0ADCBB2BF837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Problems" sheetId="1" r:id="rId1"/>
+    <sheet name="Patterns" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Question</t>
   </si>
@@ -51,33 +52,12 @@
     <t>Search in Rotated Sorted Array</t>
   </si>
   <si>
-    <t>Easy</t>
-  </si>
-  <si>
-    <t>Hard</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>GFG</t>
-  </si>
-  <si>
-    <t>LC</t>
-  </si>
-  <si>
     <t>Kth Largest/Smallest element</t>
   </si>
   <si>
     <t>Repeat and Missing Number</t>
   </si>
   <si>
-    <t>TakeYouForward</t>
-  </si>
-  <si>
-    <t>InterviewBit</t>
-  </si>
-  <si>
     <t>Two Sum</t>
   </si>
   <si>
@@ -87,18 +67,9 @@
     <t>Best Time to Buy and Sell Stock</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Meduim</t>
-  </si>
-  <si>
     <t>Container With Most Water</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>Others</t>
   </si>
   <si>
@@ -121,13 +92,58 @@
   </si>
   <si>
     <t>Merge two sorted arrays without extra space</t>
+  </si>
+  <si>
+    <t>Data Structure</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>Patterns</t>
+  </si>
+  <si>
+    <t>Binary Tree/Binary Search Tree(BST)</t>
+  </si>
+  <si>
+    <t>Kth smallest element(BST)</t>
+  </si>
+  <si>
+    <t>Kth largest element(BST)</t>
+  </si>
+  <si>
+    <t>In-order Traversal()</t>
+  </si>
+  <si>
+    <t>In-order Traversal(Reverse)</t>
+  </si>
+  <si>
+    <t>Recursive, Stack, Iterative, Morris</t>
+  </si>
+  <si>
+    <t>Flatten Binary tree to Linked list</t>
+  </si>
+  <si>
+    <t>Height of Binary Tree</t>
+  </si>
+  <si>
+    <t>Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>Maximum path sum of binary Tree</t>
+  </si>
+  <si>
+    <t>Balanced binary tree</t>
+  </si>
+  <si>
+    <t>Vertical Tree Traversal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,8 +167,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,24 +197,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -226,12 +238,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,26 +275,29 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -575,382 +614,492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555098CF-8732-4E1E-A797-9901247C4665}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E29"/>
+  <sheetPr codeName="Sheet1">
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="97.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A18"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CBB79801-D0D7-404C-8F34-D20906942510}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{45827174-B599-4F77-891A-F7B2B6FB8844}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{6E2F74AA-5177-4F0D-9BF2-7410747A7AE5}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{2A9F919C-7512-46F4-8D46-4F883163502A}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{91A25234-3846-49A8-BFCF-45B0E67D5945}"/>
-    <hyperlink ref="B11" r:id="rId6" xr:uid="{1908CD4E-5AE5-4ED3-9561-BBBB288ACB40}"/>
-    <hyperlink ref="B5" r:id="rId7" display="Buy and Sell Stocks" xr:uid="{BEAA1151-6630-4BA0-8EDF-6D20B69BAF8E}"/>
-    <hyperlink ref="B6" r:id="rId8" xr:uid="{AB30BC98-843E-4388-AF86-C17F1A5B2AEE}"/>
+    <hyperlink ref="B18" r:id="rId1" display="https://takeuforward.org/data-structure/merge-two-sorted-arrays-without-extra-space/" xr:uid="{1F1B0D60-A10F-4EDE-B132-2AD136278845}"/>
+    <hyperlink ref="B17" r:id="rId2" display="https://takeuforward.org/data-structure/length-of-the-longest-subarray-with-zero-sum/" xr:uid="{483E7229-876F-44C5-A120-93B9BF1332CB}"/>
+    <hyperlink ref="B16" r:id="rId3" display="https://takeuforward.org/data-structure/3-sum-find-triplets-that-add-up-to-a-zero/" xr:uid="{04953486-AAA5-4C46-85C4-19BAF1747D9F}"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://takeuforward.org/data-structure/longest-consecutive-sequence-in-an-array/" xr:uid="{F9D738A2-EBCB-48CF-A8E4-0BDC4341C0FF}"/>
+    <hyperlink ref="B14" r:id="rId5" display="https://takeuforward.org/arrays/longest-subarray-with-sum-k-postives-and-negatives/" xr:uid="{3F96A663-F259-47DD-9CB9-50D3771DDD2D}"/>
+    <hyperlink ref="B13" r:id="rId6" display="https://takeuforward.org/data-structure/longest-subarray-with-given-sum-k/" xr:uid="{3D923F47-C53F-45A0-A1B4-E03492FB1550}"/>
+    <hyperlink ref="B4" r:id="rId7" xr:uid="{432136EF-0602-4A0E-8387-A6D75273B492}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{88A08F9C-D11A-45ED-A7EF-E46C04E5C2AC}"/>
     <hyperlink ref="B12" r:id="rId9" xr:uid="{65187177-256A-4CE1-8952-F85FB4594CBA}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{88A08F9C-D11A-45ED-A7EF-E46C04E5C2AC}"/>
-    <hyperlink ref="B4" r:id="rId11" xr:uid="{432136EF-0602-4A0E-8387-A6D75273B492}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://takeuforward.org/data-structure/longest-subarray-with-given-sum-k/" xr:uid="{3D923F47-C53F-45A0-A1B4-E03492FB1550}"/>
-    <hyperlink ref="B14" r:id="rId13" display="https://takeuforward.org/arrays/longest-subarray-with-sum-k-postives-and-negatives/" xr:uid="{3F96A663-F259-47DD-9CB9-50D3771DDD2D}"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://takeuforward.org/data-structure/longest-consecutive-sequence-in-an-array/" xr:uid="{F9D738A2-EBCB-48CF-A8E4-0BDC4341C0FF}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://takeuforward.org/data-structure/3-sum-find-triplets-that-add-up-to-a-zero/" xr:uid="{04953486-AAA5-4C46-85C4-19BAF1747D9F}"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://takeuforward.org/data-structure/length-of-the-longest-subarray-with-zero-sum/" xr:uid="{483E7229-876F-44C5-A120-93B9BF1332CB}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://takeuforward.org/data-structure/merge-two-sorted-arrays-without-extra-space/" xr:uid="{1F1B0D60-A10F-4EDE-B132-2AD136278845}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{AB30BC98-843E-4388-AF86-C17F1A5B2AEE}"/>
+    <hyperlink ref="B5" r:id="rId11" display="Buy and Sell Stocks" xr:uid="{BEAA1151-6630-4BA0-8EDF-6D20B69BAF8E}"/>
+    <hyperlink ref="B11" r:id="rId12" xr:uid="{1908CD4E-5AE5-4ED3-9561-BBBB288ACB40}"/>
+    <hyperlink ref="B9" r:id="rId13" xr:uid="{91A25234-3846-49A8-BFCF-45B0E67D5945}"/>
+    <hyperlink ref="B8" r:id="rId14" xr:uid="{2A9F919C-7512-46F4-8D46-4F883163502A}"/>
+    <hyperlink ref="B3" r:id="rId15" xr:uid="{6E2F74AA-5177-4F0D-9BF2-7410747A7AE5}"/>
+    <hyperlink ref="B7" r:id="rId16" xr:uid="{45827174-B599-4F77-891A-F7B2B6FB8844}"/>
+    <hyperlink ref="B2" r:id="rId17" xr:uid="{CBB79801-D0D7-404C-8F34-D20906942510}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E6EAD6-325D-4CFF-AFF6-AF7B827A3B07}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A2:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[MS30082024DS] - Added few questions for Binary search Tree
</commit_message>
<xml_diff>
--- a/resources/sheets/data-structures.xlsx
+++ b/resources/sheets/data-structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasmo4a\workspace-pasmo4a\docs\data-structures\resources\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ws.intellijIDE\data-structures\resources\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33474140-0750-44CD-A916-0ADCBB2BF837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519EC3F2-D1B9-487B-A4CE-77CF5072151E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Question</t>
   </si>
@@ -106,37 +106,29 @@
     <t>Binary Tree/Binary Search Tree(BST)</t>
   </si>
   <si>
-    <t>Kth smallest element(BST)</t>
-  </si>
-  <si>
-    <t>Kth largest element(BST)</t>
-  </si>
-  <si>
     <t>In-order Traversal()</t>
   </si>
   <si>
     <t>In-order Traversal(Reverse)</t>
   </si>
   <si>
-    <t>Recursive, Stack, Iterative, Morris</t>
-  </si>
-  <si>
-    <t>Flatten Binary tree to Linked list</t>
-  </si>
-  <si>
     <t>Height of Binary Tree</t>
   </si>
   <si>
-    <t>Diameter of Binary Tree</t>
-  </si>
-  <si>
-    <t>Maximum path sum of binary Tree</t>
-  </si>
-  <si>
-    <t>Balanced binary tree</t>
-  </si>
-  <si>
-    <t>Vertical Tree Traversal</t>
+    <t>Recursive, Stack, Iterative, Morris
+Kth smallest element(BST)
+Valid Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Kth largest element(BST)
+Flatten Binary tree to Linked list</t>
+  </si>
+  <si>
+    <t>Height of Binary Tree
+Diameter of Binary Tree
+Maximum path sum of binary Tree
+Balanced binary tree
+Vertical Tree Traversal</t>
   </si>
 </sst>
 </file>
@@ -267,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -281,6 +273,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -290,14 +291,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -619,7 +620,7 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -642,7 +643,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -651,63 +652,63 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -716,49 +717,49 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -854,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,76 +877,64 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1093,11 +1082,14 @@
       <c r="C39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A2:A9"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[MSHAQ19092024DS] - Added problems on Binary Tree
</commit_message>
<xml_diff>
--- a/resources/sheets/data-structures.xlsx
+++ b/resources/sheets/data-structures.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasmo4a\workspace-pasmo4a\docs\data-structures\resources\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ws.intellijIDE\data-structures\resources\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33474140-0750-44CD-A916-0ADCBB2BF837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85632F6-F057-476D-8D01-1AF2126F633B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
-    <sheet name="Patterns" sheetId="2" r:id="rId2"/>
+    <sheet name="Trees" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Question</t>
   </si>
@@ -97,46 +97,110 @@
     <t>Data Structure</t>
   </si>
   <si>
-    <t>Problems</t>
-  </si>
-  <si>
     <t>Patterns</t>
   </si>
   <si>
-    <t>Binary Tree/Binary Search Tree(BST)</t>
-  </si>
-  <si>
-    <t>Kth smallest element(BST)</t>
-  </si>
-  <si>
-    <t>Kth largest element(BST)</t>
-  </si>
-  <si>
-    <t>In-order Traversal()</t>
-  </si>
-  <si>
-    <t>In-order Traversal(Reverse)</t>
-  </si>
-  <si>
-    <t>Recursive, Stack, Iterative, Morris</t>
-  </si>
-  <si>
-    <t>Flatten Binary tree to Linked list</t>
-  </si>
-  <si>
-    <t>Height of Binary Tree</t>
-  </si>
-  <si>
-    <t>Diameter of Binary Tree</t>
-  </si>
-  <si>
-    <t>Maximum path sum of binary Tree</t>
-  </si>
-  <si>
     <t>Balanced binary tree</t>
   </si>
   <si>
-    <t>Vertical Tree Traversal</t>
+    <t>Height of tree</t>
+  </si>
+  <si>
+    <t>Keep track of Vertex/Level</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+  </si>
+  <si>
+    <t>Right View of binary tree</t>
+  </si>
+  <si>
+    <t>Symmetry/Mirror binary tree</t>
+  </si>
+  <si>
+    <t>Boundary traversal</t>
+  </si>
+  <si>
+    <t>Left, Leaf, Right(reverse)</t>
+  </si>
+  <si>
+    <t>Compare two trees</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/description/</t>
+  </si>
+  <si>
+    <t>Zig-Zag traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height of Binary Tree
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter of Binary Tree
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum path sum of binary Tree
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-depth-of-binary-tree/description/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/diameter-of-binary-tree/description/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/binary-tree-maximum-path-sum/description/
+</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical order traversal
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top view of binary tree
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottom view of binary tree
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left view of binary tree
+</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-zigzag-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/boundary-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/vertical-order-traversal-of-a-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/top-view-of-binary-tree/1</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/bottom-view-of-binary-tree/1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-right-side-view/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/symmetric-tree/</t>
+  </si>
+  <si>
+    <t>Index based with flag</t>
   </si>
 </sst>
 </file>
@@ -202,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -262,12 +326,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -281,15 +363,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -299,6 +372,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -619,8 +721,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +744,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -651,63 +753,63 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -716,49 +818,49 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -848,258 +950,267 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E6EAD6-325D-4CFF-AFF6-AF7B827A3B07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371D7B44-8E52-4548-B94D-9B10C28F6FA8}">
   <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
+    <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="C5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="1" t="s">
+      <c r="C13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A2:A9"/>
+  <mergeCells count="3">
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="A2:A14"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{C7D7B74A-0A4F-4BD3-89CE-9A5FFC130D3D}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{FD0642C7-E064-484E-B7E3-4C80F028F74A}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{89661CB6-DE4E-43CB-8B2C-6901FA3C716C}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{2BA99058-8085-47DC-890E-A7DB68B8CAD7}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{D728E4C4-7189-414B-AC17-356DCD3E35DB}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{78BD0956-51A1-4482-B0F5-738D5BB1E3F7}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{38B408D3-B903-49BD-B0F6-46E40CEB6674}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{71CB6596-D74D-4EBC-B488-3B8336EF950A}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{D27BD383-42DA-42D8-A27F-C404EC903BF6}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{CC12621C-67BD-4406-9582-2135B35761D5}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{1DCFB45B-79B1-4443-95F0-4FACF1E72CE5}"/>
+    <hyperlink ref="C10" r:id="rId12" xr:uid="{2F1E7309-9FB8-41C3-97C0-1821B46CBF90}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{3A5B8AB2-00EB-4B45-8777-22BD15E99686}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[MSHAQ210920241256DS] - Added few problems on Binary tree and BST
</commit_message>
<xml_diff>
--- a/resources/sheets/data-structures.xlsx
+++ b/resources/sheets/data-structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ws.intellijIDE\data-structures\resources\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasmo4a\workspace-pasmo4a\docs\ws-ec\data-structures\resources\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85632F6-F057-476D-8D01-1AF2126F633B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F1A9CA-A077-470C-ABDC-DEE79F0A9904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D7F5544A-FB09-459B-9032-974DCC27F7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Question</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Balanced binary tree</t>
   </si>
   <si>
-    <t>Height of tree</t>
-  </si>
-  <si>
     <t>Keep track of Vertex/Level</t>
   </si>
   <si>
@@ -125,12 +122,6 @@
   </si>
   <si>
     <t>Compare two trees</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/same-tree/description/</t>
   </si>
   <si>
     <t>Zig-Zag traversal</t>
@@ -148,21 +139,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">https://leetcode.com/problems/maximum-depth-of-binary-tree/description/
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://leetcode.com/problems/diameter-of-binary-tree/description/
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://leetcode.com/problems/binary-tree-maximum-path-sum/description/
-</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/balanced-binary-tree/description/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vertical order traversal
 </t>
   </si>
@@ -179,28 +155,58 @@
 </t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/binary-tree-zigzag-level-order-traversal/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/boundary-of-binary-tree/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/vertical-order-traversal-of-a-binary-tree/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/problems/top-view-of-binary-tree/1</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/problems/bottom-view-of-binary-tree/1</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/binary-tree-right-side-view/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/symmetric-tree/</t>
-  </si>
-  <si>
     <t>Index based with flag</t>
+  </si>
+  <si>
+    <t>938. Range Sum of BST</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>1379. Find a Corresponding Node of a Binary Tree in a Clone of That Tree</t>
+  </si>
+  <si>
+    <t>Done pre-order traversal, wrote proper condition to check requirements, but confused how to return the node, had intuition but couldn't convert to code, should have done null check, if not null, returned node as it was answer, else the other node would've been the answer</t>
+  </si>
+  <si>
+    <t>Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Came up with logic in first 5 minutes, it was for Binary tree, here I would be traversing all the nodes, but the question was for BST, so I should have come up along with BST validation logic to improve the algorithm performance, wherein we would goto left or right subtree by comparing the roots value with given HIGH or LOW range.</t>
+  </si>
+  <si>
+    <t>BST validation</t>
+  </si>
+  <si>
+    <t>Return node but validate for null check before return</t>
+  </si>
+  <si>
+    <t>108. Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>MergeSort, Binary Search</t>
+  </si>
+  <si>
+    <t>Wrote the algorithm but used endIndex - startIndex to find middle element which gave NullPointerException while constructing the right subtree, finding middle element logic was returning 0, rather should used startIndex + endIndex, which could have retured the proper index position of right node to be created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children Sum </t>
+  </si>
+  <si>
+    <t>Height of binary tree</t>
+  </si>
+  <si>
+    <t>Top-Down</t>
+  </si>
+  <si>
+    <t>Traverse from top to down and check for validations(null and equal) and compare two sides with &amp;&amp; as two sides should be true</t>
   </si>
 </sst>
 </file>
@@ -266,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -326,30 +332,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -363,6 +351,21 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -375,32 +378,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -744,7 +741,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -753,63 +750,63 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -818,49 +815,49 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -954,21 +951,22 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" customWidth="1"/>
-    <col min="3" max="3" width="78.140625" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -976,241 +974,273 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="C3" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15" t="s">
+      <c r="C17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="C18" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="D18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="A2:A14"/>
+  <mergeCells count="6">
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{C7D7B74A-0A4F-4BD3-89CE-9A5FFC130D3D}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{FD0642C7-E064-484E-B7E3-4C80F028F74A}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{89661CB6-DE4E-43CB-8B2C-6901FA3C716C}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{2BA99058-8085-47DC-890E-A7DB68B8CAD7}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{D728E4C4-7189-414B-AC17-356DCD3E35DB}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{78BD0956-51A1-4482-B0F5-738D5BB1E3F7}"/>
-    <hyperlink ref="C13" r:id="rId7" xr:uid="{38B408D3-B903-49BD-B0F6-46E40CEB6674}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{71CB6596-D74D-4EBC-B488-3B8336EF950A}"/>
-    <hyperlink ref="C7" r:id="rId9" xr:uid="{D27BD383-42DA-42D8-A27F-C404EC903BF6}"/>
-    <hyperlink ref="C8" r:id="rId10" xr:uid="{CC12621C-67BD-4406-9582-2135B35761D5}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{1DCFB45B-79B1-4443-95F0-4FACF1E72CE5}"/>
-    <hyperlink ref="C10" r:id="rId12" xr:uid="{2F1E7309-9FB8-41C3-97C0-1821B46CBF90}"/>
-    <hyperlink ref="C12" r:id="rId13" xr:uid="{3A5B8AB2-00EB-4B45-8777-22BD15E99686}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{ADDF6A12-4467-4CE3-8A50-C8B311306E57}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{11F573D4-A44A-440B-8440-3AAD5716B497}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{6111D945-188D-4138-A2CA-44C033A2AB12}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{C9CE393C-A9AA-4E87-B271-8B952DAFCF8B}"/>
+    <hyperlink ref="B10" r:id="rId5" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{DAFF6659-FDD2-4B1C-BB00-876FE5F4858E}"/>
+    <hyperlink ref="B9" r:id="rId6" display="https://www.geeksforgeeks.org/problems/bottom-view-of-binary-tree/1" xr:uid="{83A11A67-6287-4BB0-84E2-FD3240FF3698}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.geeksforgeeks.org/problems/top-view-of-binary-tree/1" xr:uid="{98C5C2D8-986E-47B7-84F8-CFA99825B438}"/>
+    <hyperlink ref="B7" r:id="rId8" display="https://leetcode.com/problems/vertical-order-traversal-of-a-binary-tree/" xr:uid="{64AE8282-F456-4BA4-AA5C-627FD78042DE}"/>
+    <hyperlink ref="B6" r:id="rId9" xr:uid="{6372B164-2FEC-4A1D-8AED-E64CEA4AC7AC}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://leetcode.com/problems/binary-tree-maximum-path-sum/description/" xr:uid="{5E9B2604-8753-4317-BC87-F1A5DB42F060}"/>
+    <hyperlink ref="B4" r:id="rId11" display="https://leetcode.com/problems/diameter-of-binary-tree/description/" xr:uid="{B4CE3F2C-E741-4B01-A542-5386A63104E5}"/>
+    <hyperlink ref="B3" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-binary-tree/description/" xr:uid="{57E9426F-FA88-4F2A-B4CB-A99ACD3DAC44}"/>
+    <hyperlink ref="B2" r:id="rId13" xr:uid="{940B5E37-EF4A-4EC7-A357-F4DA27332410}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{35F8EF04-E558-4FF4-93C8-AF3A4AFDBD96}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{14FDF28B-FB58-425D-871F-A07F2A3990D6}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{CF3324D6-C7E4-450F-A723-C74B3448A1D8}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{2EA6A304-8CA8-468A-AB82-A8FCD0360A1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>